<commit_message>
Added headlessmode and picoContainer and threadlocal
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="134">
   <si>
     <t>testcase</t>
   </si>
@@ -366,6 +366,120 @@
   </si>
   <si>
     <t>39</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>57</t>
   </si>
 </sst>
 </file>
@@ -722,12 +836,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.88671875"/>
+    <col min="2" max="2" customWidth="true" width="14.33203125"/>
+    <col min="3" max="3" customWidth="true" width="19.5546875"/>
+    <col min="4" max="4" customWidth="true" width="14.6640625"/>
+    <col min="5" max="6" customWidth="true" width="8.88671875"/>
+    <col min="7" max="26" customWidth="true" width="8.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -28830,11 +28944,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="4" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="28" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.88671875"/>
+    <col min="2" max="4" customWidth="true" width="22.44140625"/>
+    <col min="5" max="5" customWidth="true" width="14.44140625"/>
+    <col min="6" max="6" customWidth="true" width="17.88671875"/>
+    <col min="7" max="28" customWidth="true" width="8.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1">
@@ -28866,7 +28980,7 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>32</v>
@@ -28884,7 +28998,7 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>32</v>
@@ -30014,16 +30128,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
-    <col min="10" max="28" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.33203125"/>
+    <col min="2" max="2" customWidth="true" width="19.6640625"/>
+    <col min="3" max="3" customWidth="true" width="8.6640625"/>
+    <col min="4" max="4" customWidth="true" width="24.44140625"/>
+    <col min="5" max="5" customWidth="true" width="19.6640625"/>
+    <col min="6" max="6" customWidth="true" width="8.6640625"/>
+    <col min="7" max="7" customWidth="true" width="19.6640625"/>
+    <col min="8" max="8" customWidth="true" width="20.88671875"/>
+    <col min="9" max="9" customWidth="true" width="13.88671875"/>
+    <col min="10" max="28" customWidth="true" width="8.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1">
@@ -31180,9 +31294,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" customWidth="1"/>
-    <col min="3" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.6640625"/>
+    <col min="2" max="2" customWidth="true" width="43.33203125"/>
+    <col min="3" max="26" customWidth="true" width="8.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
removed creating object for other pages
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="138">
   <si>
     <t>testcase</t>
   </si>
@@ -481,6 +481,18 @@
   <si>
     <t>57</t>
   </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
 </sst>
 </file>
 
@@ -28980,7 +28992,7 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>32</v>
@@ -28998,7 +29010,7 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>32</v>

</xml_diff>